<commit_message>
Se dejo listo el json de rappi con la info
</commit_message>
<xml_diff>
--- a/pasarporapi2.xlsx
+++ b/pasarporapi2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56978\OneDrive - Universidad Adolfo Ibanez\Desktop\Integracion Rappi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA0E2E7-0013-43FA-A0B2-046148B06F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885E2E2C-73FF-4683-BF46-6093F74C8667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{93946114-E44F-429F-B30A-1CC3411C299C}"/>
   </bookViews>
@@ -3956,8 +3956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D0049A-7F4B-4CBF-92BA-5F7769ADD917}">
   <dimension ref="A1:K390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>